<commit_message>
Worked on player controller for LO1
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F9BB91-9C1C-411A-86CA-2822BC1C11D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F90818-1CE5-4DC8-A857-7A05A022387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Learning goals" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Creating basic player controller</t>
+  </si>
+  <si>
+    <t>Working on movement</t>
+  </si>
+  <si>
+    <t>14.00 - 15.00</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +494,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>44547</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented shadows for player
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671C260D-78C9-4765-82C5-81ECA108B77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08164856-7C43-4889-89D6-162751CC8059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>2.5h</t>
+  </si>
+  <si>
+    <t>Fixed movement (left/right)</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +547,9 @@
       <c r="F7" t="s">
         <v>23</v>
       </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Worked on character controller Unreal Engine
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08164856-7C43-4889-89D6-162751CC8059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C3601A-29E1-44F3-844B-5BCDFF00C272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Learning goals" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -57,27 +66,18 @@
     <t>12.30 - 14.45</t>
   </si>
   <si>
-    <t>3.25h</t>
-  </si>
-  <si>
     <t>Exploring UE5, creating scripts</t>
   </si>
   <si>
     <t>19.00 - 21.00</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>Starting project, setting up Three.js</t>
   </si>
   <si>
     <t>17.00 - 18.00</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>Creating basic player controller</t>
   </si>
   <si>
@@ -90,16 +90,16 @@
     <t>9.45 - 11.30</t>
   </si>
   <si>
-    <t>1.75h</t>
-  </si>
-  <si>
     <t>13.30 - 16.00</t>
   </si>
   <si>
-    <t>2.5h</t>
-  </si>
-  <si>
     <t>Fixed movement (left/right)</t>
+  </si>
+  <si>
+    <t>8.45 - 12.00</t>
+  </si>
+  <si>
+    <t>Worked on character controller</t>
   </si>
 </sst>
 </file>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,13 +471,13 @@
         <v>44545</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
       <c r="O3" t="s">
         <v>8</v>
@@ -488,11 +488,11 @@
       <c r="R3" t="s">
         <v>9</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3">
+        <v>2.25</v>
+      </c>
+      <c r="U3" t="s">
         <v>10</v>
-      </c>
-      <c r="U3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -500,13 +500,25 @@
         <v>44546</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>44551</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4">
+        <v>3.25</v>
+      </c>
+      <c r="U4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -514,13 +526,13 @@
         <v>44547</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
         <v>16</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -528,13 +540,13 @@
         <v>44550</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>1.75</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -542,13 +554,19 @@
         <v>44550</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>2.5</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>SUM(F3:F7)</f>
+        <v>8.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to add physics library "Physijs"
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C3601A-29E1-44F3-844B-5BCDFF00C272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CFB16F-1104-4426-A803-83A3D3FA798E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +563,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+    </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F10">
-        <f>SUM(F3:F7)</f>
+        <f>SUM(F3:F8)</f>
         <v>8.25</v>
+      </c>
+      <c r="T10">
+        <f>SUM(T3:T4)</f>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented box trigger in UE5
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A703299-4D35-4238-A012-D2096039005E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07A4BC2-7717-456D-A42B-6D6CF1D14810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Implementing physics</t>
+  </si>
+  <si>
+    <t>15.45 - 17.00</t>
+  </si>
+  <si>
+    <t>Implemented box trigger</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +558,18 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
+      <c r="Q5" s="1">
+        <v>44552</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5">
+        <v>1.25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
@@ -623,8 +641,8 @@
         <v>27</v>
       </c>
       <c r="T10">
-        <f>SUM(T3:T4)</f>
-        <v>5.5</v>
+        <f>SUM(T3:T5)</f>
+        <v>6.75</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on door animation/opening
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77100679-4CAD-490B-A5E8-C25D11ED2CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B58B5-9265-47F9-AAC9-6994FE2BC86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Recreated project after crash</t>
+  </si>
+  <si>
+    <t>10.30 - 13.00</t>
+  </si>
+  <si>
+    <t>Continuing level</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +757,20 @@
         <v>39</v>
       </c>
     </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1">
+        <v>44568</v>
+      </c>
+      <c r="R12" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12">
+        <v>2.5</v>
+      </c>
+      <c r="U12" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F14">
         <f>SUM(F3:F10)</f>
@@ -759,8 +779,8 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T15">
-        <f>SUM(T3:T11)</f>
-        <v>19.75</v>
+        <f>SUM(T3:T12)</f>
+        <v>22.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented physics in threejs game, worked on UE level
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADAA804-66F1-4CFF-97A8-377E094DA577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAF2BEB-CCDB-4FE7-BA49-2C0BCC64C3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Implemented game over trigger</t>
+  </si>
+  <si>
+    <t>Added lava</t>
+  </si>
+  <si>
+    <t>13.30 - 15.00</t>
+  </si>
+  <si>
+    <t>After a (too) long break from this LO, trying to implement physics again</t>
   </si>
 </sst>
 </file>
@@ -505,7 +514,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,6 +771,18 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>44572</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11">
+        <v>1.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
       <c r="Q11" s="1">
         <v>44567</v>
       </c>
@@ -804,10 +825,6 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F14">
-        <f>SUM(F3:F10)</f>
-        <v>13.5</v>
-      </c>
       <c r="Q14" s="1">
         <v>44569</v>
       </c>
@@ -835,10 +852,31 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1">
+        <v>44571</v>
+      </c>
+      <c r="R16" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16">
+        <v>2.5</v>
+      </c>
+      <c r="U16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="22" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f>SUM(F3:F11)</f>
+        <v>15</v>
+      </c>
       <c r="T22">
-        <f>SUM(T3:T15)</f>
-        <v>26.25</v>
+        <f>SUM(T3:T16)</f>
+        <v>28.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on level & jumping
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAF2BEB-CCDB-4FE7-BA49-2C0BCC64C3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99680E80-5A7A-4315-A239-54C7A62F8703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>Added lava</t>
-  </si>
-  <si>
-    <t>13.30 - 15.00</t>
   </si>
   <si>
     <t>After a (too) long break from this LO, trying to implement physics again</t>
@@ -514,7 +511,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,13 +772,13 @@
         <v>44572</v>
       </c>
       <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11" t="s">
         <v>49</v>
-      </c>
-      <c r="F11">
-        <v>1.5</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
       </c>
       <c r="Q11" s="1">
         <v>44567</v>
@@ -872,7 +869,7 @@
     <row r="22" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F22">
         <f>SUM(F3:F11)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T22">
         <f>SUM(T3:T16)</f>

</xml_diff>

<commit_message>
Working on 2nd puzzle
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99680E80-5A7A-4315-A239-54C7A62F8703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E4E0E-8BF0-4B18-AC7D-E528C49EE4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Learning goal 2</t>
   </si>
   <si>
-    <t>(Website)</t>
-  </si>
-  <si>
     <t>(Unreal Engine)</t>
   </si>
   <si>
@@ -184,6 +181,24 @@
   </si>
   <si>
     <t>After a (too) long break from this LO, trying to implement physics again</t>
+  </si>
+  <si>
+    <t>9.00 - 12.30</t>
+  </si>
+  <si>
+    <t>8.30 - 12.00</t>
+  </si>
+  <si>
+    <t>13.00 - 18.30</t>
+  </si>
+  <si>
+    <t>Implemented physics, jumping, cleaned up code</t>
+  </si>
+  <si>
+    <t>12.30 - 16.00</t>
+  </si>
+  <si>
+    <t>(Web game)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +526,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,34 +570,34 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1">
         <v>44545</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="1">
         <v>44545</v>
       </c>
       <c r="R3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T3">
         <v>2.25</v>
       </c>
       <c r="U3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -590,25 +605,25 @@
         <v>44546</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" s="1">
         <v>44551</v>
       </c>
       <c r="R4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T4">
         <v>3.25</v>
       </c>
       <c r="U4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -616,25 +631,25 @@
         <v>44547</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="1">
         <v>44552</v>
       </c>
       <c r="R5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T5">
         <v>1.25</v>
       </c>
       <c r="U5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -642,25 +657,25 @@
         <v>44550</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>1.75</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="1">
         <v>44565</v>
       </c>
       <c r="R6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T6">
         <v>2</v>
       </c>
       <c r="U6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -668,25 +683,25 @@
         <v>44550</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>2.5</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q7" s="1">
         <v>44565</v>
       </c>
       <c r="R7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T7">
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -694,25 +709,25 @@
         <v>44551</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="1">
         <v>44566</v>
       </c>
       <c r="R8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T8">
         <v>3.5</v>
       </c>
       <c r="U8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -720,25 +735,25 @@
         <v>44552</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>2.5</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="1">
         <v>44566</v>
       </c>
       <c r="R9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T9">
         <v>1.5</v>
       </c>
       <c r="U9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -746,25 +761,25 @@
         <v>44552</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>1.75</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q10" s="1">
         <v>44567</v>
       </c>
       <c r="R10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T10">
         <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -772,53 +787,77 @@
         <v>44572</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11">
         <v>2.5</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q11" s="1">
         <v>44567</v>
       </c>
       <c r="R11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T11">
         <v>3</v>
       </c>
       <c r="U11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>44573</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12">
+        <v>5.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
       <c r="Q12" s="1">
         <v>44568</v>
       </c>
       <c r="R12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T12">
         <v>2.5</v>
       </c>
       <c r="U12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>44574</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>3.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
       <c r="Q13" s="1">
         <v>44568</v>
       </c>
       <c r="R13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -826,13 +865,13 @@
         <v>44569</v>
       </c>
       <c r="R14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T14">
         <v>2</v>
       </c>
       <c r="U14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -840,13 +879,13 @@
         <v>44570</v>
       </c>
       <c r="R15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -854,26 +893,51 @@
         <v>44571</v>
       </c>
       <c r="R16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T16">
         <v>2.5</v>
       </c>
       <c r="U16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="22" spans="6:20" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1">
+        <v>44573</v>
+      </c>
+      <c r="R17" t="s">
+        <v>49</v>
+      </c>
+      <c r="T17">
+        <v>3.5</v>
+      </c>
+      <c r="U17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1">
+        <v>44574</v>
+      </c>
+      <c r="R18" t="s">
+        <v>50</v>
+      </c>
+      <c r="T18">
+        <v>3.5</v>
+      </c>
+      <c r="U18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F22">
-        <f>SUM(F3:F11)</f>
-        <v>16</v>
+        <f>SUM(F3:F13)</f>
+        <v>25</v>
       </c>
       <c r="T22">
-        <f>SUM(T3:T16)</f>
-        <v>28.75</v>
+        <f>SUM(T3:T18)</f>
+        <v>35.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made planning until deadlines
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F57F26-5593-433D-AE8F-1DFBC2D4741E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888BB07-75E3-45EA-95B4-56505A9BF1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>13.00 - 16.00</t>
+  </si>
+  <si>
+    <t>9.00 - 12.00</t>
+  </si>
+  <si>
+    <t>9.00  - 12.00</t>
+  </si>
+  <si>
+    <t>13.00 - 17.00</t>
   </si>
 </sst>
 </file>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,6 +870,15 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>44579</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
       <c r="Q14" s="1">
         <v>44569</v>
       </c>
@@ -875,6 +893,15 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>44580</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
       <c r="Q15" s="1">
         <v>44570</v>
       </c>
@@ -889,6 +916,15 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>44581</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
       <c r="Q16" s="1">
         <v>44571</v>
       </c>
@@ -902,7 +938,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>44587</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
       <c r="Q17" s="1">
         <v>44573</v>
       </c>
@@ -916,7 +961,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>44588</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
       <c r="Q18" s="1">
         <v>44574</v>
       </c>
@@ -930,14 +984,107 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f>SUM(F3:F13)</f>
-        <v>25</v>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>44589</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>44580</v>
+      </c>
+      <c r="R19" t="s">
+        <v>56</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>44592</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>44581</v>
+      </c>
+      <c r="R20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>44593</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>44588</v>
+      </c>
+      <c r="R21" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1">
+        <v>44589</v>
+      </c>
+      <c r="R22" t="s">
+        <v>55</v>
       </c>
       <c r="T22">
-        <f>SUM(T3:T18)</f>
-        <v>35.75</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f>SUM(F3:F21)</f>
+        <v>54</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>44592</v>
+      </c>
+      <c r="R23" t="s">
+        <v>55</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1">
+        <v>44593</v>
+      </c>
+      <c r="R24" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <f>SUM(T3:T24)</f>
+        <v>53.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on menu - level transition
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881406D-2E97-47CD-A750-4DEE99BD2443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ABFAA5-F0C8-4751-B79F-AE3C67F25F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -214,6 +214,21 @@
   </si>
   <si>
     <t>12.00 - 20.00</t>
+  </si>
+  <si>
+    <t>12.00  - 19.30</t>
+  </si>
+  <si>
+    <t>12.00 - 21.00</t>
+  </si>
+  <si>
+    <t>11.00 - 13.30</t>
+  </si>
+  <si>
+    <t>Menu - level transition</t>
+  </si>
+  <si>
+    <t>14.00 - 17.00</t>
   </si>
 </sst>
 </file>
@@ -538,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,53 +926,80 @@
       <c r="F15">
         <v>2.75</v>
       </c>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1">
+        <v>44570</v>
+      </c>
+      <c r="R15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>44587</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
       <c r="Q16" s="1">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="R16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="U16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>44588</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17">
+        <v>7.5</v>
+      </c>
       <c r="Q17" s="1">
-        <v>44571</v>
+        <v>44573</v>
       </c>
       <c r="R17" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="T17">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="U17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
-        <v>44587</v>
+        <v>44589</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q18" s="1">
-        <v>44573</v>
+        <v>44574</v>
       </c>
       <c r="R18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T18">
         <v>3.5</v>
@@ -968,7 +1010,7 @@
     </row>
     <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
-        <v>44588</v>
+        <v>44592</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
@@ -977,21 +1019,21 @@
         <v>4</v>
       </c>
       <c r="Q19" s="1">
-        <v>44574</v>
+        <v>44589</v>
       </c>
       <c r="R19" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="T19">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="U19" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <v>44589</v>
+        <v>44593</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
@@ -999,74 +1041,65 @@
       <c r="F20">
         <v>4</v>
       </c>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1">
+        <v>44592</v>
+      </c>
+      <c r="R20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>44592</v>
+        <v>44594</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>44593</v>
+      </c>
+      <c r="R21" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
-        <v>44593</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="Q22" s="1">
+        <v>44594</v>
+      </c>
+      <c r="R22" t="s">
+        <v>55</v>
+      </c>
+      <c r="T22">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q23" s="1">
-        <v>44589</v>
-      </c>
-      <c r="R23" t="s">
-        <v>55</v>
-      </c>
-      <c r="T23">
-        <v>3</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F24">
-        <f>SUM(F3:F22)</f>
-        <v>55.25</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>44592</v>
-      </c>
-      <c r="R24" t="s">
-        <v>55</v>
-      </c>
+        <f>SUM(F3:F23)</f>
+        <v>57.75</v>
+      </c>
+      <c r="Q24" s="1"/>
       <c r="T24">
-        <v>3</v>
+        <f>SUM(T3:T22)</f>
+        <v>47.25</v>
       </c>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="Q25" s="1">
-        <v>44593</v>
-      </c>
-      <c r="R25" t="s">
-        <v>55</v>
-      </c>
-      <c r="T25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="T27">
-        <f>SUM(T3:T25)</f>
-        <v>44.75</v>
-      </c>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Q26" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Implemented full scene transitions after winning/losing
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ABFAA5-F0C8-4751-B79F-AE3C67F25F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455386F1-1184-49FE-BAE3-95CD22693C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Learning goals" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Hour registration Nils Meijer EC2MV.Ea</t>
   </si>
@@ -204,9 +204,6 @@
     <t>9.00 - 12.00</t>
   </si>
   <si>
-    <t>13.00 - 17.00</t>
-  </si>
-  <si>
     <t>Vertical UI movement</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>12.00  - 19.30</t>
   </si>
   <si>
-    <t>12.00 - 21.00</t>
-  </si>
-  <si>
     <t>11.00 - 13.30</t>
   </si>
   <si>
@@ -229,6 +223,36 @@
   </si>
   <si>
     <t>14.00 - 17.00</t>
+  </si>
+  <si>
+    <t>10.00 - 16.00</t>
+  </si>
+  <si>
+    <t>12.00 - 15.00</t>
+  </si>
+  <si>
+    <t>12.00 - 14.00</t>
+  </si>
+  <si>
+    <t>Full scene transitions winning/losing</t>
+  </si>
+  <si>
+    <t>Writing reflection</t>
+  </si>
+  <si>
+    <t>Implemented scene loading</t>
+  </si>
+  <si>
+    <t>Cleaning code, working on scene loading</t>
+  </si>
+  <si>
+    <t>level, UI movement</t>
+  </si>
+  <si>
+    <t>Added tweening lib.  Implemented door functionality, replaced HTML UI with THREE text</t>
+  </si>
+  <si>
+    <t>Working on physics/contact materials</t>
   </si>
 </sst>
 </file>
@@ -556,7 +580,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +925,7 @@
         <v>3.5</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q14" s="1">
         <v>44569</v>
@@ -921,10 +945,13 @@
         <v>44579</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15">
         <v>2.75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
       </c>
       <c r="Q15" s="1">
         <v>44570</v>
@@ -944,10 +971,13 @@
         <v>44587</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16">
         <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
       </c>
       <c r="Q16" s="1">
         <v>44571</v>
@@ -967,10 +997,13 @@
         <v>44588</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <v>7.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
       </c>
       <c r="Q17" s="1">
         <v>44573</v>
@@ -990,10 +1023,13 @@
         <v>44589</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F18">
         <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
       </c>
       <c r="Q18" s="1">
         <v>44574</v>
@@ -1013,53 +1049,57 @@
         <v>44592</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
       </c>
       <c r="Q19" s="1">
         <v>44589</v>
       </c>
       <c r="R19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T19">
         <v>2.5</v>
       </c>
       <c r="U19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
+        <v>44594</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" s="1">
         <v>44593</v>
       </c>
-      <c r="D20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>44592</v>
-      </c>
       <c r="R20" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="T20">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="U20" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+      <c r="C21" s="1"/>
+      <c r="Q21" s="1">
         <v>44594</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>44593</v>
       </c>
       <c r="R21" t="s">
         <v>55</v>
@@ -1067,18 +1107,13 @@
       <c r="T21">
         <v>3</v>
       </c>
+      <c r="U21" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="22" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-      <c r="Q22" s="1">
-        <v>44594</v>
-      </c>
-      <c r="R22" t="s">
-        <v>55</v>
-      </c>
-      <c r="T22">
-        <v>3</v>
-      </c>
+      <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
@@ -1087,12 +1122,12 @@
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F24">
         <f>SUM(F3:F23)</f>
-        <v>57.75</v>
+        <v>58.75</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="T24">
         <f>SUM(T3:T22)</f>
-        <v>47.25</v>
+        <v>43.25</v>
       </c>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">

</xml_diff>